<commit_message>
Optimizer testing for new processes
</commit_message>
<xml_diff>
--- a/efficiency_testing/sim_1_10/Optimizer_Testing_NN_propensity.xlsx
+++ b/efficiency_testing/sim_1_10/Optimizer_Testing_NN_propensity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcg\Google Drive\MasterThesis\dml_est_general\efficiency_testing\sim_1_10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BDEEE92-946F-4F46-979A-9A173418EEAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC586F90-54F3-421C-BEA6-830CBF942891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{6A5FBCD0-C166-4D81-9F0C-49E81C69DCD3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6A5FBCD0-C166-4D81-9F0C-49E81C69DCD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Single_Layer" sheetId="4" r:id="rId1"/>
@@ -574,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0013E5D1-B0BE-4F3F-93C2-18356612F2E4}">
   <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1134,6 +1134,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
     <mergeCell ref="Q3:R3"/>
     <mergeCell ref="Q4:R4"/>
     <mergeCell ref="Q5:R5"/>
@@ -1150,17 +1161,6 @@
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1171,8 +1171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{166A5B32-9AC9-417B-B8AA-7D7202DC2B5D}">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1588,22 +1588,54 @@
       <c r="B11" s="1">
         <v>0.01</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
+      <c r="C11" s="1">
+        <v>29.8</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E11" s="1">
+        <v>29.95</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G11" s="1">
+        <v>30.77</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="I11" s="1">
+        <v>29.73</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.27</v>
+      </c>
+      <c r="K11" s="1">
+        <v>31.78</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="M11" s="1">
+        <v>31.91</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="O11" s="1">
+        <v>31.65</v>
+      </c>
+      <c r="P11" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>32.76</v>
+      </c>
+      <c r="R11" s="1">
+        <v>0.28999999999999998</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -2101,22 +2133,54 @@
       <c r="B26" s="1">
         <v>0.01</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
+      <c r="C26" s="1">
+        <v>30.35</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.31</v>
+      </c>
+      <c r="E26" s="1">
+        <v>31.95</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="G26" s="1">
+        <v>31.48</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0.31</v>
+      </c>
+      <c r="I26" s="1">
+        <v>32.22</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0.31</v>
+      </c>
+      <c r="K26" s="1">
+        <v>32.29</v>
+      </c>
+      <c r="L26" s="1">
+        <v>0.31</v>
+      </c>
+      <c r="M26" s="1">
+        <v>32.44</v>
+      </c>
+      <c r="N26" s="1">
+        <v>0.31</v>
+      </c>
+      <c r="O26" s="1">
+        <v>31.25</v>
+      </c>
+      <c r="P26" s="1">
+        <v>0.31</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>33.4</v>
+      </c>
+      <c r="R26" s="1">
+        <v>0.31</v>
+      </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -2212,6 +2276,44 @@
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="Q3:R3"/>
@@ -2228,44 +2330,6 @@
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added analysis of all DGPs, changes in hyperparam files due to formatting of excel needed for preparation of tables in thesis
</commit_message>
<xml_diff>
--- a/efficiency_testing/sim_1_10/Optimizer_Testing_NN_propensity.xlsx
+++ b/efficiency_testing/sim_1_10/Optimizer_Testing_NN_propensity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcg\Google Drive\MasterThesis\dml_est_general\efficiency_testing\sim_1_10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC586F90-54F3-421C-BEA6-830CBF942891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960B1EE3-5C16-4761-ABBB-BCCE788EC3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6A5FBCD0-C166-4D81-9F0C-49E81C69DCD3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{6A5FBCD0-C166-4D81-9F0C-49E81C69DCD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Single_Layer" sheetId="4" r:id="rId1"/>
@@ -64,9 +64,6 @@
     <t>Time</t>
   </si>
   <si>
-    <t>RMSE</t>
-  </si>
-  <si>
     <t>Learning_rate</t>
   </si>
   <si>
@@ -140,6 +137,9 @@
   </si>
   <si>
     <t>Min LogLoss &amp; min time</t>
+  </si>
+  <si>
+    <t>Activation functions</t>
   </si>
 </sst>
 </file>
@@ -241,11 +241,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -258,6 +257,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0013E5D1-B0BE-4F3F-93C2-18356612F2E4}">
   <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,462 +588,462 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="4">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="4">
-        <v>1</v>
-      </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="4">
-        <v>1</v>
-      </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="4">
-        <v>1</v>
-      </c>
-      <c r="J3" s="5"/>
-      <c r="K3" s="4">
-        <v>1</v>
-      </c>
-      <c r="L3" s="5"/>
-      <c r="M3" s="4">
-        <v>1</v>
-      </c>
-      <c r="N3" s="5"/>
-      <c r="O3" s="4">
-        <v>1</v>
-      </c>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="4">
-        <v>1</v>
-      </c>
-      <c r="R3" s="5"/>
+      <c r="A3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="3">
+        <v>1</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="K3" s="3">
+        <v>1</v>
+      </c>
+      <c r="L3" s="4"/>
+      <c r="M3" s="3">
+        <v>1</v>
+      </c>
+      <c r="N3" s="4"/>
+      <c r="O3" s="3">
+        <v>1</v>
+      </c>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="3">
+        <v>1</v>
+      </c>
+      <c r="R3" s="4"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="4"/>
+      <c r="M4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" s="4"/>
+      <c r="O4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="R4" s="4"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" s="5"/>
-      <c r="M4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="N4" s="5"/>
-      <c r="O4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="R4" s="5"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="4">
+      <c r="B5" s="6"/>
+      <c r="C5" s="3">
         <v>8</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="4">
+      <c r="D5" s="4"/>
+      <c r="E5" s="3">
         <v>16</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="4">
+      <c r="F5" s="4"/>
+      <c r="G5" s="3">
         <v>32</v>
       </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="4">
+      <c r="H5" s="4"/>
+      <c r="I5" s="3">
         <v>64</v>
       </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="4">
+      <c r="J5" s="4"/>
+      <c r="K5" s="3">
         <v>8</v>
       </c>
-      <c r="L5" s="5"/>
-      <c r="M5" s="4">
+      <c r="L5" s="4"/>
+      <c r="M5" s="3">
         <v>16</v>
       </c>
-      <c r="N5" s="5"/>
-      <c r="O5" s="4">
+      <c r="N5" s="4"/>
+      <c r="O5" s="3">
         <v>32</v>
       </c>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="4">
+      <c r="P5" s="4"/>
+      <c r="Q5" s="3">
         <v>64</v>
       </c>
-      <c r="R5" s="5"/>
+      <c r="R5" s="4"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1">
         <v>0.01</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="7">
         <v>6.27</v>
       </c>
-      <c r="D7" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="E7" s="1">
+      <c r="D7" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="E7" s="7">
         <v>5.0199999999999996</v>
       </c>
-      <c r="F7" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="G7" s="1">
+      <c r="F7" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="G7" s="7">
         <v>4.5199999999999996</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="7">
         <v>0.27</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="7">
         <v>4.13</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="7">
         <v>0.28999999999999998</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="7">
         <v>10.58</v>
       </c>
-      <c r="L7" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="M7" s="1">
+      <c r="L7" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="M7" s="7">
         <v>8.27</v>
       </c>
-      <c r="N7" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="O7" s="1">
+      <c r="N7" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="O7" s="7">
         <v>7.06</v>
       </c>
-      <c r="P7" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="Q7" s="3">
+      <c r="P7" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="Q7" s="8">
         <v>6.63</v>
       </c>
-      <c r="R7" s="3">
+      <c r="R7" s="8">
         <v>0.24</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1">
         <v>0.01</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="7">
         <v>11.43</v>
       </c>
-      <c r="D8" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="E8" s="1">
+      <c r="D8" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="E8" s="7">
         <v>7.99</v>
       </c>
-      <c r="F8" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="G8" s="1">
+      <c r="F8" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="G8" s="7">
         <v>6.97</v>
       </c>
-      <c r="H8" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="I8" s="1">
+      <c r="H8" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="I8" s="7">
         <v>5.54</v>
       </c>
-      <c r="J8" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="K8" s="1">
+      <c r="J8" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="K8" s="7">
         <v>22.58</v>
       </c>
-      <c r="L8" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="M8" s="1">
+      <c r="L8" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="M8" s="7">
         <v>18.25</v>
       </c>
-      <c r="N8" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="O8" s="1">
+      <c r="N8" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="O8" s="7">
         <v>15.35</v>
       </c>
-      <c r="P8" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="Q8" s="1">
+      <c r="P8" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="Q8" s="7">
         <v>14.01</v>
       </c>
-      <c r="R8" s="1">
+      <c r="R8" s="7">
         <v>0.24</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1">
         <v>0.1</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="7">
         <v>10.050000000000001</v>
       </c>
-      <c r="D9" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="E9" s="1">
+      <c r="D9" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="E9" s="7">
         <v>8.26</v>
       </c>
-      <c r="F9" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="G9" s="1">
+      <c r="F9" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="G9" s="7">
         <v>6.73</v>
       </c>
-      <c r="H9" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="I9" s="1">
+      <c r="H9" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="I9" s="7">
         <v>6.78</v>
       </c>
-      <c r="J9" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="K9" s="1">
+      <c r="J9" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="K9" s="7">
         <v>32.57</v>
       </c>
-      <c r="L9" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="M9" s="1">
+      <c r="L9" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="M9" s="7">
         <v>34.04</v>
       </c>
-      <c r="N9" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="O9" s="1">
+      <c r="N9" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="O9" s="7">
         <v>34.06</v>
       </c>
-      <c r="P9" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="Q9" s="1">
+      <c r="P9" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="Q9" s="7">
         <v>20.62</v>
       </c>
-      <c r="R9" s="1">
+      <c r="R9" s="7">
         <v>0.25</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1">
         <v>0.01</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="7">
         <v>5.09</v>
       </c>
-      <c r="D10" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="E10" s="1">
+      <c r="D10" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="E10" s="7">
         <v>4.62</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="7">
         <v>0.27</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="7">
         <v>4.24</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="7">
         <v>0.27</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="7">
         <v>3.94</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="7">
         <v>0.28999999999999998</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="7">
         <v>8.7100000000000009</v>
       </c>
-      <c r="L10" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="M10" s="1">
+      <c r="L10" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="M10" s="7">
         <v>7.48</v>
       </c>
-      <c r="N10" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="O10" s="1">
+      <c r="N10" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="O10" s="7">
         <v>6.85</v>
       </c>
-      <c r="P10" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="Q10" s="1">
+      <c r="P10" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="Q10" s="7">
         <v>6.58</v>
       </c>
-      <c r="R10" s="1">
+      <c r="R10" s="7">
         <v>0.25</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="1">
         <v>0.01</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="7">
         <v>32.99</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="7">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="7">
         <v>32.76</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="7">
         <v>0.27</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="7">
         <v>32.08</v>
       </c>
-      <c r="H11" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="I11" s="1">
+      <c r="H11" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="I11" s="7">
         <v>32.18</v>
       </c>
-      <c r="J11" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="K11" s="1">
+      <c r="J11" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="K11" s="7">
         <v>32.64</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L11" s="7">
         <v>0.3</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M11" s="7">
         <v>32.51</v>
       </c>
-      <c r="N11" s="1">
+      <c r="N11" s="7">
         <v>0.3</v>
       </c>
-      <c r="O11" s="1">
+      <c r="O11" s="7">
         <v>32.700000000000003</v>
       </c>
-      <c r="P11" s="1">
+      <c r="P11" s="7">
         <v>0.3</v>
       </c>
-      <c r="Q11" s="1">
+      <c r="Q11" s="7">
         <v>32.6</v>
       </c>
-      <c r="R11" s="1">
+      <c r="R11" s="7">
         <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13">
         <f>MIN(D7:D11)</f>
@@ -1079,7 +1080,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14">
         <f>MIN(D13:R13)</f>
@@ -1088,7 +1089,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" t="e">
         <f>IF(_xlfn.MINIFS(C7:C11,D7:D11,$D$14) = 0, NA(), _xlfn.MINIFS(C7:C11,D7:D11,$D$14))</f>
@@ -1125,7 +1126,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" cm="1">
         <f t="array" ref="D16">MIN(IF(ISNUMBER(D15:R15),D15:R15,""))</f>
@@ -1134,17 +1135,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
     <mergeCell ref="Q3:R3"/>
     <mergeCell ref="Q4:R4"/>
     <mergeCell ref="Q5:R5"/>
@@ -1161,6 +1151,17 @@
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1171,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{166A5B32-9AC9-417B-B8AA-7D7202DC2B5D}">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1184,462 +1185,462 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="3">
+        <v>2</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="3">
+        <v>2</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="K3" s="3">
+        <v>2</v>
+      </c>
+      <c r="L3" s="4"/>
+      <c r="M3" s="3">
+        <v>2</v>
+      </c>
+      <c r="N3" s="4"/>
+      <c r="O3" s="3">
+        <v>2</v>
+      </c>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="3">
+        <v>2</v>
+      </c>
+      <c r="R3" s="4"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="4">
-        <v>2</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="4">
-        <v>2</v>
-      </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="4">
-        <v>2</v>
-      </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="4">
-        <v>2</v>
-      </c>
-      <c r="J3" s="5"/>
-      <c r="K3" s="4">
-        <v>2</v>
-      </c>
-      <c r="L3" s="5"/>
-      <c r="M3" s="4">
-        <v>2</v>
-      </c>
-      <c r="N3" s="5"/>
-      <c r="O3" s="4">
-        <v>2</v>
-      </c>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="4">
-        <v>2</v>
-      </c>
-      <c r="R3" s="5"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="4"/>
+      <c r="M4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" s="4"/>
+      <c r="O4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4" s="4"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="4" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L4" s="5"/>
-      <c r="M4" s="4" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="5"/>
-      <c r="O4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="R4" s="5"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="4" t="s">
+      <c r="L5" s="4"/>
+      <c r="M5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="4" t="s">
+      <c r="N5" s="4"/>
+      <c r="O5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="4" t="s">
+      <c r="P5" s="4"/>
+      <c r="Q5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5" s="5"/>
-      <c r="M5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N5" s="5"/>
-      <c r="O5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="R5" s="5"/>
+      <c r="R5" s="4"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1">
         <v>0.01</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="7">
         <v>5.48</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="7">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="7">
         <v>4.96</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="7">
         <v>0.3</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="7">
         <v>4.9400000000000004</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="7">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="7">
         <v>4.41</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="7">
         <v>0.34</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="7">
         <v>6.63</v>
       </c>
-      <c r="L7" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="M7" s="1">
+      <c r="L7" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="M7" s="7">
         <v>6.46</v>
       </c>
-      <c r="N7" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="O7" s="1">
+      <c r="N7" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="O7" s="7">
         <v>6.12</v>
       </c>
-      <c r="P7" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="Q7" s="1">
+      <c r="P7" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="Q7" s="7">
         <v>5.82</v>
       </c>
-      <c r="R7" s="1">
+      <c r="R7" s="7">
         <v>0.26</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1">
         <v>0.01</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="7">
         <v>7.67</v>
       </c>
-      <c r="D8" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="E8" s="1">
+      <c r="D8" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="E8" s="7">
         <v>6.44</v>
       </c>
-      <c r="F8" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="G8" s="1">
+      <c r="F8" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="G8" s="7">
         <v>7.87</v>
       </c>
-      <c r="H8" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="I8" s="1">
+      <c r="H8" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="I8" s="7">
         <v>6.32</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="7">
         <v>0.27</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="7">
         <v>11.73</v>
       </c>
-      <c r="L8" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="M8" s="1">
+      <c r="L8" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="M8" s="7">
         <v>11.11</v>
       </c>
-      <c r="N8" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="O8" s="1">
+      <c r="N8" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="O8" s="7">
         <v>10.74</v>
       </c>
-      <c r="P8" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="Q8" s="1">
+      <c r="P8" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="Q8" s="7">
         <v>9.93</v>
       </c>
-      <c r="R8" s="1">
+      <c r="R8" s="7">
         <v>0.24</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1">
         <v>0.1</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="7">
         <v>8.09</v>
       </c>
-      <c r="D9" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="E9" s="1">
+      <c r="D9" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="E9" s="7">
         <v>6.67</v>
       </c>
-      <c r="F9" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="G9" s="1">
+      <c r="F9" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="G9" s="7">
         <v>7.97</v>
       </c>
-      <c r="H9" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="I9" s="1">
+      <c r="H9" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="I9" s="7">
         <v>7.36</v>
       </c>
-      <c r="J9" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="K9" s="1">
+      <c r="J9" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="K9" s="7">
         <v>22.17</v>
       </c>
-      <c r="L9" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="M9" s="1">
+      <c r="L9" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="M9" s="7">
         <v>16.84</v>
       </c>
-      <c r="N9" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="O9" s="1">
+      <c r="N9" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="O9" s="7">
         <v>17.73</v>
       </c>
-      <c r="P9" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="Q9" s="1">
+      <c r="P9" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="Q9" s="7">
         <v>18.05</v>
       </c>
-      <c r="R9" s="1">
+      <c r="R9" s="7">
         <v>0.24</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1">
         <v>0.01</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="7">
         <v>5.14</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="7">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="7">
         <v>4.6500000000000004</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="7">
         <v>0.28999999999999998</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="7">
         <v>5.03</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="7">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="7">
         <v>4.5199999999999996</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="7">
         <v>0.31</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="7">
         <v>7.8</v>
       </c>
-      <c r="L10" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="M10" s="1">
+      <c r="L10" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="M10" s="7">
         <v>6.44</v>
       </c>
-      <c r="N10" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="O10" s="1">
+      <c r="N10" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="O10" s="7">
         <v>6.64</v>
       </c>
-      <c r="P10" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="Q10" s="1">
+      <c r="P10" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="Q10" s="7">
         <v>6.48</v>
       </c>
-      <c r="R10" s="1">
+      <c r="R10" s="7">
         <v>0.26</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="1">
         <v>0.01</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="7">
         <v>29.8</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="7">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="7">
         <v>29.95</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="7">
         <v>0.28000000000000003</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="7">
         <v>30.77</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="7">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="7">
         <v>29.73</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="7">
         <v>0.27</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="7">
         <v>31.78</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L11" s="7">
         <v>0.3</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M11" s="7">
         <v>31.91</v>
       </c>
-      <c r="N11" s="1">
+      <c r="N11" s="7">
         <v>0.3</v>
       </c>
-      <c r="O11" s="1">
+      <c r="O11" s="7">
         <v>31.65</v>
       </c>
-      <c r="P11" s="1">
+      <c r="P11" s="7">
         <v>0.3</v>
       </c>
-      <c r="Q11" s="1">
+      <c r="Q11" s="7">
         <v>32.76</v>
       </c>
-      <c r="R11" s="1">
+      <c r="R11" s="7">
         <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13">
         <f>MIN(D7:D11)</f>
@@ -1676,7 +1677,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14">
         <f>MIN(D13:R13)</f>
@@ -1685,7 +1686,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" t="e">
         <f>IF(_xlfn.MINIFS(C7:C11,D7:D11,$D$14) = 0, NA(), _xlfn.MINIFS(C7:C11,D7:D11,$D$14))</f>
@@ -1722,7 +1723,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" cm="1">
         <f t="array" ref="D16">MIN(IF(ISNUMBER(D15:R15),D15:R15,""))</f>
@@ -1733,458 +1734,458 @@
       <c r="A17" s="2"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="3">
+        <v>2</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="3">
+        <v>2</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="3">
+        <v>2</v>
+      </c>
+      <c r="H18" s="4"/>
+      <c r="I18" s="3">
+        <v>2</v>
+      </c>
+      <c r="J18" s="4"/>
+      <c r="K18" s="3">
+        <v>2</v>
+      </c>
+      <c r="L18" s="4"/>
+      <c r="M18" s="3">
+        <v>2</v>
+      </c>
+      <c r="N18" s="4"/>
+      <c r="O18" s="3">
+        <v>2</v>
+      </c>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="3">
+        <v>2</v>
+      </c>
+      <c r="R18" s="4"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="4">
-        <v>2</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="4">
-        <v>2</v>
-      </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="4">
-        <v>2</v>
-      </c>
-      <c r="H18" s="5"/>
-      <c r="I18" s="4">
-        <v>2</v>
-      </c>
-      <c r="J18" s="5"/>
-      <c r="K18" s="4">
-        <v>2</v>
-      </c>
-      <c r="L18" s="5"/>
-      <c r="M18" s="4">
-        <v>2</v>
-      </c>
-      <c r="N18" s="5"/>
-      <c r="O18" s="4">
-        <v>2</v>
-      </c>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="4">
-        <v>2</v>
-      </c>
-      <c r="R18" s="5"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
+      <c r="B19" s="6"/>
+      <c r="C19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="4"/>
+      <c r="I19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" s="4"/>
+      <c r="K19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L19" s="4"/>
+      <c r="M19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N19" s="4"/>
+      <c r="O19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="R19" s="4"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H19" s="5"/>
-      <c r="I19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J19" s="5"/>
-      <c r="K19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L19" s="5"/>
-      <c r="M19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="N19" s="5"/>
-      <c r="O19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="R19" s="5"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="4" t="s">
+      <c r="B20" s="6"/>
+      <c r="C20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="4" t="s">
+      <c r="F20" s="4"/>
+      <c r="G20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="5"/>
-      <c r="G20" s="4" t="s">
+      <c r="H20" s="4"/>
+      <c r="I20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H20" s="5"/>
-      <c r="I20" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J20" s="5"/>
-      <c r="K20" s="4" t="s">
+      <c r="J20" s="4"/>
+      <c r="K20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L20" s="4"/>
+      <c r="M20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L20" s="5"/>
-      <c r="M20" s="4" t="s">
+      <c r="N20" s="4"/>
+      <c r="O20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N20" s="5"/>
-      <c r="O20" s="4" t="s">
+      <c r="P20" s="4"/>
+      <c r="Q20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="R20" s="5"/>
+      <c r="R20" s="4"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>1</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="M21" s="1" t="s">
         <v>1</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="O21" s="1" t="s">
         <v>1</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="Q21" s="1" t="s">
         <v>1</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B22" s="1">
         <v>0.01</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="7">
         <v>5.95</v>
       </c>
-      <c r="D22" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="E22" s="1">
+      <c r="D22" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="E22" s="7">
         <v>4.87</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="7">
         <v>0.27</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="7">
         <v>4.8899999999999997</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22" s="7">
         <v>0.27</v>
       </c>
-      <c r="I22" s="1">
+      <c r="I22" s="7">
         <v>4.83</v>
       </c>
-      <c r="J22" s="1">
+      <c r="J22" s="7">
         <v>0.28000000000000003</v>
       </c>
-      <c r="K22" s="1">
+      <c r="K22" s="7">
         <v>8.41</v>
       </c>
-      <c r="L22" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="M22" s="1">
+      <c r="L22" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="M22" s="7">
         <v>6.78</v>
       </c>
-      <c r="N22" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="O22" s="1">
+      <c r="N22" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="O22" s="7">
         <v>7.85</v>
       </c>
-      <c r="P22" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="Q22" s="1">
+      <c r="P22" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="Q22" s="7">
         <v>6.9</v>
       </c>
-      <c r="R22" s="1">
+      <c r="R22" s="7">
         <v>0.25</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23" s="1">
         <v>0.01</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="7">
         <v>10.56</v>
       </c>
-      <c r="D23" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="E23" s="1">
+      <c r="D23" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="E23" s="7">
         <v>8.64</v>
       </c>
-      <c r="F23" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="G23" s="1">
+      <c r="F23" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="G23" s="7">
         <v>8.51</v>
       </c>
-      <c r="H23" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="I23" s="1">
+      <c r="H23" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="I23" s="7">
         <v>6.8</v>
       </c>
-      <c r="J23" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="K23" s="1">
+      <c r="J23" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="K23" s="7">
         <v>16.5</v>
       </c>
-      <c r="L23" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="M23" s="1">
+      <c r="L23" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="M23" s="7">
         <v>14.4</v>
       </c>
-      <c r="N23" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="O23" s="1">
+      <c r="N23" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="O23" s="7">
         <v>16.38</v>
       </c>
-      <c r="P23" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="Q23" s="1">
+      <c r="P23" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="Q23" s="7">
         <v>14.21</v>
       </c>
-      <c r="R23" s="1">
+      <c r="R23" s="7">
         <v>0.24</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B24" s="1">
         <v>0.1</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="7">
         <v>16.28</v>
       </c>
-      <c r="D24" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="E24" s="1">
+      <c r="D24" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="E24" s="7">
         <v>13.31</v>
       </c>
-      <c r="F24" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="G24" s="1">
+      <c r="F24" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="G24" s="7">
         <v>14.73</v>
       </c>
-      <c r="H24" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="I24" s="1">
+      <c r="H24" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="I24" s="7">
         <v>12.28</v>
       </c>
-      <c r="J24" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="K24" s="1">
+      <c r="J24" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="K24" s="7">
         <v>31.76</v>
       </c>
-      <c r="L24" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="M24" s="1">
+      <c r="L24" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="M24" s="7">
         <v>34.89</v>
       </c>
-      <c r="N24" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="O24" s="1">
+      <c r="N24" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="O24" s="7">
         <v>32.020000000000003</v>
       </c>
-      <c r="P24" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="Q24" s="1">
+      <c r="P24" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="Q24" s="7">
         <v>33.909999999999997</v>
       </c>
-      <c r="R24" s="1">
+      <c r="R24" s="7">
         <v>0.24</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B25" s="1">
         <v>0.01</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="7">
         <v>5.52</v>
       </c>
-      <c r="D25" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="E25" s="1">
+      <c r="D25" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="E25" s="7">
         <v>5.0199999999999996</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25" s="7">
         <v>0.27</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="7">
         <v>4.75</v>
       </c>
-      <c r="H25" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="I25" s="1">
+      <c r="H25" s="7">
+        <v>0.26</v>
+      </c>
+      <c r="I25" s="7">
         <v>4.76</v>
       </c>
-      <c r="J25" s="1">
+      <c r="J25" s="7">
         <v>0.27</v>
       </c>
-      <c r="K25" s="1">
+      <c r="K25" s="7">
         <v>8.4600000000000009</v>
       </c>
-      <c r="L25" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="M25" s="1">
+      <c r="L25" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="M25" s="7">
         <v>7.4</v>
       </c>
-      <c r="N25" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="O25" s="1">
+      <c r="N25" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="O25" s="7">
         <v>7.4</v>
       </c>
-      <c r="P25" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="Q25" s="1">
+      <c r="P25" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="Q25" s="7">
         <v>7.32</v>
       </c>
-      <c r="R25" s="1">
+      <c r="R25" s="7">
         <v>0.24</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B26" s="1">
         <v>0.01</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="7">
         <v>30.35</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="7">
         <v>0.31</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26" s="7">
         <v>31.95</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26" s="7">
         <v>0.3</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26" s="7">
         <v>31.48</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H26" s="7">
         <v>0.31</v>
       </c>
-      <c r="I26" s="1">
+      <c r="I26" s="7">
         <v>32.22</v>
       </c>
-      <c r="J26" s="1">
+      <c r="J26" s="7">
         <v>0.31</v>
       </c>
-      <c r="K26" s="1">
+      <c r="K26" s="7">
         <v>32.29</v>
       </c>
-      <c r="L26" s="1">
+      <c r="L26" s="7">
         <v>0.31</v>
       </c>
-      <c r="M26" s="1">
+      <c r="M26" s="7">
         <v>32.44</v>
       </c>
-      <c r="N26" s="1">
+      <c r="N26" s="7">
         <v>0.31</v>
       </c>
-      <c r="O26" s="1">
+      <c r="O26" s="7">
         <v>31.25</v>
       </c>
-      <c r="P26" s="1">
+      <c r="P26" s="7">
         <v>0.31</v>
       </c>
-      <c r="Q26" s="1">
+      <c r="Q26" s="7">
         <v>33.4</v>
       </c>
-      <c r="R26" s="1">
+      <c r="R26" s="7">
         <v>0.31</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D28">
         <f>MIN(D22:D26)</f>
@@ -2221,7 +2222,7 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D29">
         <f>MIN(D28:R28)</f>
@@ -2230,7 +2231,7 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D30">
         <f>IF(_xlfn.MINIFS(C22:C26,D22:D26,$D$14) = 0, NA(), _xlfn.MINIFS(C22:C26,D22:D26,$D$14))</f>
@@ -2267,7 +2268,7 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D31">
         <f t="array" ref="D31">MIN(IF(ISNUMBER(D30:R30),D30:R30,""))</f>
@@ -2276,44 +2277,6 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="Q3:R3"/>
@@ -2330,6 +2293,44 @@
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>